<commit_message>
0.0.12: Throw IllegalArgumentException instead of NullPointerException, on delegate issue errors. And delete some redundant debug logs.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoValueObjectKtResourceBundle.xlsx
+++ b/meta/program/BlancoValueObjectKtResourceBundle.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1EAEE64-590F-E846-B27D-72D25302576D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB505C5-6332-0643-A649-F10CF4BD52E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="111">
   <si>
     <t>説明</t>
     <rPh sb="0" eb="2">
@@ -611,6 +613,17 @@
   </si>
   <si>
     <t>META2XML.ELEMENT_COMMON_KT</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>XML2SOURCE_FILE.ERR007</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>クラス名[{0}]の委譲フィールド[{1}]の型名が指定されていません。</t>
+    <rPh sb="10" eb="12">
+      <t xml:space="preserve">イジョウ </t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1443,10 +1456,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I87"/>
+  <dimension ref="A1:I88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1613,7 +1626,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="28">
-        <f t="shared" ref="A17:A80" si="0">A16+1</f>
+        <f t="shared" ref="A17:A81" si="0">A16+1</f>
         <v>3</v>
       </c>
       <c r="B17" s="23"/>
@@ -2175,8 +2188,12 @@
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="B55" s="23"/>
-      <c r="C55" s="20"/>
+      <c r="B55" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="C55" s="20" t="s">
+        <v>110</v>
+      </c>
       <c r="D55" s="21"/>
       <c r="E55" s="21"/>
       <c r="F55" s="21"/>
@@ -2184,15 +2201,11 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="28">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="B56" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="C56" s="20" t="s">
-        <v>77</v>
-      </c>
+        <f>A54+1</f>
+        <v>41</v>
+      </c>
+      <c r="B56" s="23"/>
+      <c r="C56" s="20"/>
       <c r="D56" s="21"/>
       <c r="E56" s="21"/>
       <c r="F56" s="21"/>
@@ -2201,13 +2214,13 @@
     <row r="57" spans="1:7">
       <c r="A57" s="28">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B57" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C57" s="20" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="D57" s="21"/>
       <c r="E57" s="21"/>
@@ -2217,13 +2230,13 @@
     <row r="58" spans="1:7">
       <c r="A58" s="28">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B58" s="23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C58" s="20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D58" s="21"/>
       <c r="E58" s="21"/>
@@ -2233,10 +2246,14 @@
     <row r="59" spans="1:7">
       <c r="A59" s="28">
         <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="B59" s="23"/>
-      <c r="C59" s="20"/>
+        <v>44</v>
+      </c>
+      <c r="B59" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C59" s="20" t="s">
+        <v>58</v>
+      </c>
       <c r="D59" s="21"/>
       <c r="E59" s="21"/>
       <c r="F59" s="21"/>
@@ -2245,14 +2262,10 @@
     <row r="60" spans="1:7">
       <c r="A60" s="28">
         <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="B60" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="C60" s="20" t="s">
-        <v>78</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B60" s="23"/>
+      <c r="C60" s="20"/>
       <c r="D60" s="21"/>
       <c r="E60" s="21"/>
       <c r="F60" s="21"/>
@@ -2261,13 +2274,13 @@
     <row r="61" spans="1:7">
       <c r="A61" s="28">
         <f t="shared" si="0"/>
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B61" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C61" s="20" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="D61" s="21"/>
       <c r="E61" s="21"/>
@@ -2277,13 +2290,13 @@
     <row r="62" spans="1:7">
       <c r="A62" s="28">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B62" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C62" s="20" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="D62" s="21"/>
       <c r="E62" s="21"/>
@@ -2293,10 +2306,14 @@
     <row r="63" spans="1:7">
       <c r="A63" s="28">
         <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="B63" s="23"/>
-      <c r="C63" s="20"/>
+        <v>48</v>
+      </c>
+      <c r="B63" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C63" s="20" t="s">
+        <v>79</v>
+      </c>
       <c r="D63" s="21"/>
       <c r="E63" s="21"/>
       <c r="F63" s="21"/>
@@ -2305,14 +2322,10 @@
     <row r="64" spans="1:7">
       <c r="A64" s="28">
         <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="B64" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="C64" s="20" t="s">
-        <v>80</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="B64" s="23"/>
+      <c r="C64" s="20"/>
       <c r="D64" s="21"/>
       <c r="E64" s="21"/>
       <c r="F64" s="21"/>
@@ -2321,13 +2334,13 @@
     <row r="65" spans="1:7">
       <c r="A65" s="28">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B65" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C65" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D65" s="21"/>
       <c r="E65" s="21"/>
@@ -2337,13 +2350,13 @@
     <row r="66" spans="1:7">
       <c r="A66" s="28">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B66" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C66" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D66" s="21"/>
       <c r="E66" s="21"/>
@@ -2353,13 +2366,13 @@
     <row r="67" spans="1:7">
       <c r="A67" s="28">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B67" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C67" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D67" s="21"/>
       <c r="E67" s="21"/>
@@ -2369,10 +2382,14 @@
     <row r="68" spans="1:7">
       <c r="A68" s="28">
         <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-      <c r="B68" s="23"/>
-      <c r="C68" s="20"/>
+        <v>53</v>
+      </c>
+      <c r="B68" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C68" s="20" t="s">
+        <v>83</v>
+      </c>
       <c r="D68" s="21"/>
       <c r="E68" s="21"/>
       <c r="F68" s="21"/>
@@ -2381,14 +2398,10 @@
     <row r="69" spans="1:7">
       <c r="A69" s="28">
         <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-      <c r="B69" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="C69" s="20" t="s">
-        <v>84</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="B69" s="23"/>
+      <c r="C69" s="20"/>
       <c r="D69" s="21"/>
       <c r="E69" s="21"/>
       <c r="F69" s="21"/>
@@ -2397,13 +2410,13 @@
     <row r="70" spans="1:7">
       <c r="A70" s="28">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B70" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C70" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D70" s="21"/>
       <c r="E70" s="21"/>
@@ -2413,13 +2426,13 @@
     <row r="71" spans="1:7">
       <c r="A71" s="28">
         <f t="shared" si="0"/>
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B71" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C71" s="20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D71" s="21"/>
       <c r="E71" s="21"/>
@@ -2429,13 +2442,13 @@
     <row r="72" spans="1:7">
       <c r="A72" s="28">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B72" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C72" s="20" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="D72" s="21"/>
       <c r="E72" s="21"/>
@@ -2445,10 +2458,14 @@
     <row r="73" spans="1:7">
       <c r="A73" s="28">
         <f t="shared" si="0"/>
-        <v>59</v>
-      </c>
-      <c r="B73" s="23"/>
-      <c r="C73" s="20"/>
+        <v>58</v>
+      </c>
+      <c r="B73" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="C73" s="20" t="s">
+        <v>70</v>
+      </c>
       <c r="D73" s="21"/>
       <c r="E73" s="21"/>
       <c r="F73" s="21"/>
@@ -2457,14 +2474,10 @@
     <row r="74" spans="1:7">
       <c r="A74" s="28">
         <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="B74" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="C74" s="20" t="s">
-        <v>87</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="B74" s="23"/>
+      <c r="C74" s="20"/>
       <c r="D74" s="21"/>
       <c r="E74" s="21"/>
       <c r="F74" s="21"/>
@@ -2473,10 +2486,14 @@
     <row r="75" spans="1:7">
       <c r="A75" s="28">
         <f t="shared" si="0"/>
-        <v>61</v>
-      </c>
-      <c r="B75" s="23"/>
-      <c r="C75" s="20"/>
+        <v>60</v>
+      </c>
+      <c r="B75" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="C75" s="20" t="s">
+        <v>87</v>
+      </c>
       <c r="D75" s="21"/>
       <c r="E75" s="21"/>
       <c r="F75" s="21"/>
@@ -2485,12 +2502,10 @@
     <row r="76" spans="1:7">
       <c r="A76" s="28">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B76" s="23"/>
-      <c r="C76" s="20" t="s">
-        <v>72</v>
-      </c>
+      <c r="C76" s="20"/>
       <c r="D76" s="21"/>
       <c r="E76" s="21"/>
       <c r="F76" s="21"/>
@@ -2499,11 +2514,11 @@
     <row r="77" spans="1:7">
       <c r="A77" s="28">
         <f t="shared" si="0"/>
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B77" s="23"/>
       <c r="C77" s="20" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="D77" s="21"/>
       <c r="E77" s="21"/>
@@ -2513,11 +2528,11 @@
     <row r="78" spans="1:7">
       <c r="A78" s="28">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B78" s="23"/>
       <c r="C78" s="20" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="D78" s="21"/>
       <c r="E78" s="21"/>
@@ -2527,10 +2542,12 @@
     <row r="79" spans="1:7">
       <c r="A79" s="28">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B79" s="23"/>
-      <c r="C79" s="20"/>
+      <c r="C79" s="20" t="s">
+        <v>72</v>
+      </c>
       <c r="D79" s="21"/>
       <c r="E79" s="21"/>
       <c r="F79" s="21"/>
@@ -2539,14 +2556,10 @@
     <row r="80" spans="1:7">
       <c r="A80" s="28">
         <f t="shared" si="0"/>
-        <v>66</v>
-      </c>
-      <c r="B80" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="C80" s="20" t="s">
-        <v>89</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="B80" s="23"/>
+      <c r="C80" s="20"/>
       <c r="D80" s="21"/>
       <c r="E80" s="21"/>
       <c r="F80" s="21"/>
@@ -2554,14 +2567,14 @@
     </row>
     <row r="81" spans="1:7">
       <c r="A81" s="28">
-        <f>A80+1</f>
-        <v>67</v>
+        <f t="shared" si="0"/>
+        <v>66</v>
       </c>
       <c r="B81" s="23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C81" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D81" s="21"/>
       <c r="E81" s="21"/>
@@ -2570,14 +2583,14 @@
     </row>
     <row r="82" spans="1:7">
       <c r="A82" s="28">
-        <f>A81+1</f>
-        <v>68</v>
+        <f t="shared" ref="A82:A87" si="1">A81+1</f>
+        <v>67</v>
       </c>
       <c r="B82" s="23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C82" s="20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D82" s="21"/>
       <c r="E82" s="21"/>
@@ -2586,14 +2599,14 @@
     </row>
     <row r="83" spans="1:7">
       <c r="A83" s="28">
-        <f>A82+1</f>
-        <v>69</v>
+        <f t="shared" si="1"/>
+        <v>68</v>
       </c>
       <c r="B83" s="23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C83" s="20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D83" s="21"/>
       <c r="E83" s="21"/>
@@ -2602,14 +2615,14 @@
     </row>
     <row r="84" spans="1:7">
       <c r="A84" s="28">
-        <f>A83+1</f>
-        <v>70</v>
+        <f t="shared" si="1"/>
+        <v>69</v>
       </c>
       <c r="B84" s="23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C84" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D84" s="21"/>
       <c r="E84" s="21"/>
@@ -2618,14 +2631,14 @@
     </row>
     <row r="85" spans="1:7">
       <c r="A85" s="28">
-        <f>A84+1</f>
-        <v>71</v>
+        <f t="shared" si="1"/>
+        <v>70</v>
       </c>
       <c r="B85" s="23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C85" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D85" s="21"/>
       <c r="E85" s="21"/>
@@ -2634,14 +2647,14 @@
     </row>
     <row r="86" spans="1:7">
       <c r="A86" s="28">
-        <f>A85+1</f>
-        <v>72</v>
+        <f t="shared" si="1"/>
+        <v>71</v>
       </c>
       <c r="B86" s="23" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C86" s="20" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="D86" s="21"/>
       <c r="E86" s="21"/>
@@ -2649,13 +2662,29 @@
       <c r="G86" s="22"/>
     </row>
     <row r="87" spans="1:7">
-      <c r="A87" s="29"/>
-      <c r="B87" s="24"/>
-      <c r="C87" s="25"/>
-      <c r="D87" s="26"/>
-      <c r="E87" s="26"/>
-      <c r="F87" s="26"/>
-      <c r="G87" s="27"/>
+      <c r="A87" s="28">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="B87" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C87" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D87" s="21"/>
+      <c r="E87" s="21"/>
+      <c r="F87" s="21"/>
+      <c r="G87" s="22"/>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88" s="29"/>
+      <c r="B88" s="24"/>
+      <c r="C88" s="25"/>
+      <c r="D88" s="26"/>
+      <c r="E88" s="26"/>
+      <c r="F88" s="26"/>
+      <c r="G88" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>